<commit_message>
Favori ürünler sorunu düzeltildi
</commit_message>
<xml_diff>
--- a/Notlar/Mevcut özellikler.xlsx
+++ b/Notlar/Mevcut özellikler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehme\Desktop\Projem\masamenu\Notlar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6530AD55-667E-4420-AA4E-00A1812B1FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B6EFDC-8B75-406B-A313-2D030615AD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="İŞLETME ÖZELLİKLER" sheetId="1" r:id="rId1"/>
@@ -536,46 +536,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="162"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="162"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -654,6 +614,66 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="162"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="162"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="162"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -738,26 +758,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="162"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -778,7 +778,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -787,14 +787,14 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
+        <sz val="16"/>
         <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <charset val="162"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,28 +810,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A59ACE81-0606-4026-B46E-366D37A40265}" name="Tablo3" displayName="Tablo3" ref="A1:E34" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A59ACE81-0606-4026-B46E-366D37A40265}" name="Tablo3" displayName="Tablo3" ref="A1:E34" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E34" xr:uid="{A59ACE81-0606-4026-B46E-366D37A40265}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1C86C3B5-B827-4D94-8C8D-2E5EE9148E35}" name="NO" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{CE68D3B6-C068-4FDF-8E7D-9FEB0D38D1D5}" name="ÖZELLİKLER" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{BF0B9FC7-A4DA-4EF4-ACE8-FA045B26F13B}" name="DURUM" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{531896DD-2F64-4962-B0A3-3F6E8DD64429}" name="ORAN" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{E114EAD6-00A4-4F86-851D-BCCA25882E38}" name="AÇIKLMA VE DOSYA YOLU" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{1C86C3B5-B827-4D94-8C8D-2E5EE9148E35}" name="NO" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{CE68D3B6-C068-4FDF-8E7D-9FEB0D38D1D5}" name="ÖZELLİKLER" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{BF0B9FC7-A4DA-4EF4-ACE8-FA045B26F13B}" name="DURUM" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{531896DD-2F64-4962-B0A3-3F6E8DD64429}" name="ORAN" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E114EAD6-00A4-4F86-851D-BCCA25882E38}" name="AÇIKLMA VE DOSYA YOLU" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DA8B4E4B-EE47-4E33-AD35-315B6407ABCB}" name="Tablo4" displayName="Tablo4" ref="A1:E29" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DA8B4E4B-EE47-4E33-AD35-315B6407ABCB}" name="Tablo4" displayName="Tablo4" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E29" xr:uid="{DA8B4E4B-EE47-4E33-AD35-315B6407ABCB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2C77BA40-7BBD-455A-8A99-386B41CF1EF5}" name="NO" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{4C9F5A7D-0463-4586-BFC3-643183E3E563}" name="ÖZELLİKLER" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{ED39C769-2B70-4857-9A88-6A6BFB49B3E0}" name="DURUM" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{3463E2F7-289D-48EF-B322-D6D79EFEECFD}" name="ORAN" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D819BFDA-2BAC-425C-A26F-6F0DBE954A6E}" name="AÇIKLMA VE DOSYA YOU" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2C77BA40-7BBD-455A-8A99-386B41CF1EF5}" name="NO" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4C9F5A7D-0463-4586-BFC3-643183E3E563}" name="ÖZELLİKLER" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{ED39C769-2B70-4857-9A88-6A6BFB49B3E0}" name="DURUM" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3463E2F7-289D-48EF-B322-D6D79EFEECFD}" name="ORAN" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D819BFDA-2BAC-425C-A26F-6F0DBE954A6E}" name="AÇIKLMA VE DOSYA YOU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1105,7 +1105,7 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1846,8 +1846,8 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -2038,7 +2038,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D11" s="13">
         <v>0.6</v>

</xml_diff>

<commit_message>
Müşteri tarfında favorilerden sipariş verme aktif edildi
</commit_message>
<xml_diff>
--- a/Notlar/Mevcut özellikler.xlsx
+++ b/Notlar/Mevcut özellikler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehme\Desktop\Projem\masamenu\Notlar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B6EFDC-8B75-406B-A313-2D030615AD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3068F9-DB97-438E-AA6C-54EA43CA8FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +445,14 @@
       <family val="1"/>
       <charset val="162"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -466,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -507,6 +515,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2037,7 +2048,7 @@
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="13">

</xml_diff>

<commit_message>
QR kod ile menüye yönlendirme düzeltiliyır
</commit_message>
<xml_diff>
--- a/Notlar/Mevcut özellikler.xlsx
+++ b/Notlar/Mevcut özellikler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehme\Desktop\Projem\masamenu\Notlar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3068F9-DB97-438E-AA6C-54EA43CA8FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BE3EF8-1728-427E-A0DF-3EBA3376586A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>